<commit_message>
updates to 2017 household survey script
</commit_message>
<xml_diff>
--- a/2017/summary/destination_simple.xlsx
+++ b/2017/summary/destination_simple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travel-studies\2017\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B12CA4-72D2-4056-9CAF-2CA054797D30}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1CB583-FB16-4463-BCA4-DA19F0C8B7C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{5730C50B-1828-491D-A1B6-3C75870F173B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Went home</t>
   </si>
@@ -110,10 +110,19 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Social/Recreation</t>
-  </si>
-  <si>
     <t>Destination purpose</t>
+  </si>
+  <si>
+    <t>Drop off/Pick up</t>
+  </si>
+  <si>
+    <t>Social/Recreation/Eat Meal</t>
+  </si>
+  <si>
+    <t>Health and Exercise</t>
+  </si>
+  <si>
+    <t>Errands</t>
   </si>
 </sst>
 </file>
@@ -490,16 +499,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD34FCD-CF27-468E-A70A-B202D7E73D23}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -526,7 +537,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -574,7 +585,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -582,7 +593,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -590,7 +601,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -598,7 +609,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -606,7 +617,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -614,7 +625,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,7 +633,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -630,7 +641,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -646,7 +657,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -654,7 +665,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
including code to also summarize 2014
</commit_message>
<xml_diff>
--- a/2017/summary/destination_simple.xlsx
+++ b/2017/summary/destination_simple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\travel-studies\2017\summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1CB583-FB16-4463-BCA4-DA19F0C8B7C4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353D3F73-8CC1-4E99-9EFE-79BD5329918D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{5730C50B-1828-491D-A1B6-3C75870F173B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Went home</t>
   </si>
@@ -104,25 +104,13 @@
     <t>Work</t>
   </si>
   <si>
-    <t>Shop</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Destination purpose</t>
   </si>
   <si>
-    <t>Drop off/Pick up</t>
-  </si>
-  <si>
-    <t>Social/Recreation/Eat Meal</t>
-  </si>
-  <si>
-    <t>Health and Exercise</t>
-  </si>
-  <si>
-    <t>Errands</t>
+    <t>Recreation/Eat Meal</t>
+  </si>
+  <si>
+    <t>Errands and Shopping</t>
   </si>
 </sst>
 </file>
@@ -500,7 +488,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +498,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -537,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,7 +565,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +573,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +581,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +589,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,7 +597,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -617,7 +605,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -625,7 +613,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -633,7 +621,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +629,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +637,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -657,7 +645,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -665,7 +653,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -673,7 +661,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>